<commit_message>
Have begun learning how to use tidy models. Cleaned up data for use with tidy models.
</commit_message>
<xml_diff>
--- a/Variable List.xlsx
+++ b/Variable List.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
   <si>
     <t>Variable</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">% White, Not Hispanic</t>
   </si>
   <si>
+    <t xml:space="preserve">PEP (1991 - 2024); IPUMS Time Series (1980, 1990)</t>
+  </si>
+  <si>
     <t xml:space="preserve">% of total population that is White.</t>
   </si>
   <si>
@@ -86,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">Shannon Index of Diversity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEP (1991 - 2024); IPUMS Time Series (1980, 1990)</t>
   </si>
   <si>
     <r>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">% in poverty</t>
   </si>
   <si>
-    <t xml:space="preserve">SAIPE (1989 - 2024); IPUMS Time Series (1980, 1990, 2000, 2010-2023)</t>
+    <t xml:space="preserve">SAIPE (1989 - 2024); IPUMS Time Series (1980)</t>
   </si>
   <si>
     <t xml:space="preserve">Poverty ratios</t>
@@ -967,7 +967,7 @@
 The 75th percentile for home value</t>
   </si>
   <si>
-    <t xml:space="preserve">1980 has different valus for housing. Additionally, it is missing the 25th percentile and 75th percentile values.</t>
+    <t xml:space="preserve">From 2009 to 2014, the max value is $1,000,000 and above while from 2015 and onwards additional categories are added ($1,000,000 - $1,499,999; $1,500,000 - $1,999,999; $2,000,000 and above). 1980 has different values for housing. Additionally, it is missing the 25th percentile and 75th percentile values.</t>
   </si>
   <si>
     <t xml:space="preserve">White (not Hispanic) median home value</t>
@@ -1028,7 +1028,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">ACS (2009 - 2023); IPUMS Time Series (1980, 1990); </t>
+      <t xml:space="preserve">ACS (2009; 2011 - 2019; 2021 -2023); IPUMS Time Series (1980, 1990; 2010; 2020); </t>
     </r>
     <r>
       <rPr>
@@ -1056,7 +1056,7 @@
     <t xml:space="preserve">% female-headed alone households</t>
   </si>
   <si>
-    <t xml:space="preserve">ACS (2009 - 2023); IPUMS Time Series (1980, 1990, 2000)</t>
+    <t xml:space="preserve">ACS (2009; 2011 - 2019; 2021 -2023); IPUMS Time Series (1980, 1990; 2000; 2010; 2020)</t>
   </si>
   <si>
     <t xml:space="preserve">% of all households that are female-headed with no spouse present and with related children in the household</t>
@@ -1289,34 +1289,6 @@
   </si>
   <si>
     <t xml:space="preserve">Children can live with a grandparent, another relative, a foster parent, or some unreleated person. Parents include biological parents, step parents, and adoptive parents.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">SAIPE (1989 - 2024);</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="2"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">IPUMS (1980)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">% of White (not Hispanic) children in poverty</t>
@@ -1701,8 +1673,8 @@
       <top style="thin">
         <color theme="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -1711,9 +1683,9 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -1722,11 +1694,11 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top/>
+      <top style="none"/>
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="none"/>
@@ -1763,6 +1735,13 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1774,13 +1753,7 @@
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="3" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1832,18 +1805,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2391,117 +2362,131 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" ht="28.5">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" ht="28.5">
       <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" ht="28.5">
       <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" ht="28.5">
       <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" ht="42.75">
       <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" ht="42.75">
       <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" ht="171">
       <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="7" t="s">
         <v>23</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
@@ -2512,14 +2497,16 @@
       <c r="E9" s="3">
         <v>1</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" ht="171">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>23</v>
+      <c r="B10" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2" t="s">
@@ -2528,49 +2515,59 @@
       <c r="E10" s="3">
         <v>1</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" ht="28.5">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="3"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="3"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" ht="42.75">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" ht="28.5">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" ht="99.75">
       <c r="A15" s="2" t="s">
@@ -2586,19 +2583,23 @@
       <c r="E15" s="3">
         <v>7</v>
       </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" ht="42.75">
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" ht="28.5">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" ht="28.5">
       <c r="A17" s="2" t="s">
@@ -2613,7 +2614,9 @@
       <c r="E17" s="3">
         <v>1</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" ht="185.25">
       <c r="A18" s="2" t="s">
@@ -2631,7 +2634,9 @@
       <c r="E18" s="3">
         <v>14</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" ht="28.5">
       <c r="A19" s="2" t="s">
@@ -2643,47 +2648,53 @@
       <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" ht="85.5">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="13" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="3">
         <v>6</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" ht="28.5">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="10">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3"/>
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" ht="42.75">
       <c r="A22" s="2" t="s">
@@ -2698,7 +2709,9 @@
       <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" ht="42.75">
       <c r="A23" s="2" t="s">
@@ -2713,7 +2726,9 @@
       <c r="E23" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" ht="28.5">
       <c r="A24" s="2" t="s">
@@ -2725,7 +2740,9 @@
       <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" ht="42.75">
       <c r="A25" s="2" t="s">
@@ -2743,7 +2760,9 @@
       <c r="E25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" ht="28.5">
       <c r="A26" s="2" t="s">
@@ -2759,7 +2778,9 @@
       <c r="E26" s="3">
         <v>1</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" ht="28.5">
       <c r="A27" s="2" t="s">
@@ -2772,7 +2793,9 @@
       <c r="E27" s="3">
         <v>1</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" ht="42.75">
       <c r="A28" s="2" t="s">
@@ -2787,7 +2810,9 @@
       <c r="E28" s="3">
         <v>1</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" ht="28.5">
       <c r="A29" s="2" t="s">
@@ -2799,7 +2824,9 @@
       <c r="E29" s="3">
         <v>1</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" ht="42.75">
       <c r="A30" s="2" t="s">
@@ -2817,7 +2844,9 @@
       <c r="E30" s="3">
         <v>1</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" ht="28.5">
       <c r="A31" s="2" t="s">
@@ -2832,7 +2861,9 @@
       <c r="E31" s="3">
         <v>1</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" ht="28.5">
       <c r="A32" s="2" t="s">
@@ -2847,7 +2878,9 @@
       <c r="E32" s="3">
         <v>1</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" ht="57">
       <c r="A33" s="2" t="s">
@@ -2862,7 +2895,9 @@
       <c r="E33" s="3">
         <v>1</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" ht="28.5">
       <c r="A34" s="2" t="s">
@@ -2877,7 +2912,9 @@
       <c r="E34" s="3">
         <v>1</v>
       </c>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" ht="57">
       <c r="A35" s="2" t="s">
@@ -2895,7 +2932,9 @@
       <c r="E35" s="3">
         <v>1</v>
       </c>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" ht="28.5">
       <c r="A36" s="2" t="s">
@@ -2913,7 +2952,9 @@
       <c r="E36" s="3">
         <v>1</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" ht="185.25">
       <c r="A37" s="2" t="s">
@@ -2931,7 +2972,9 @@
       <c r="E37" s="3">
         <v>14</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="38" ht="185.25">
       <c r="A38" s="2" t="s">
@@ -2949,7 +2992,9 @@
       <c r="E38" s="3">
         <v>14</v>
       </c>
-      <c r="F38" s="3"/>
+      <c r="F38" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" ht="185.25">
       <c r="A39" s="2" t="s">
@@ -2967,7 +3012,9 @@
       <c r="E39" s="3">
         <v>14</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="40" ht="57">
       <c r="A40" s="2" t="s">
@@ -2982,7 +3029,9 @@
       <c r="E40" s="3">
         <v>4</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" ht="57">
       <c r="A41" s="2" t="s">
@@ -2997,7 +3046,9 @@
       <c r="E41" s="3">
         <v>4</v>
       </c>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" ht="57">
       <c r="A42" s="2" t="s">
@@ -3015,7 +3066,9 @@
       <c r="E42" s="3">
         <v>4</v>
       </c>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="43" ht="57">
       <c r="A43" s="2" t="s">
@@ -3030,7 +3083,9 @@
       <c r="E43" s="3">
         <v>4</v>
       </c>
-      <c r="F43" s="3"/>
+      <c r="F43" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="44" ht="42.75">
       <c r="A44" s="2" t="s">
@@ -3048,7 +3103,9 @@
       <c r="E44" s="3">
         <v>1</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" ht="28.5">
       <c r="A45" s="2" t="s">
@@ -3063,7 +3120,9 @@
       <c r="E45" s="3">
         <v>1</v>
       </c>
-      <c r="F45" s="3"/>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" ht="42.75">
       <c r="A46" s="2" t="s">
@@ -3078,7 +3137,9 @@
       <c r="E46" s="3">
         <v>1</v>
       </c>
-      <c r="F46" s="3"/>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" ht="28.5">
       <c r="A47" s="2" t="s">
@@ -3093,7 +3154,9 @@
       <c r="E47" s="3">
         <v>1</v>
       </c>
-      <c r="F47" s="3"/>
+      <c r="F47" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" ht="28.5">
       <c r="A48" s="2" t="s">
@@ -3108,7 +3171,9 @@
       <c r="E48" s="3">
         <v>1</v>
       </c>
-      <c r="F48" s="3"/>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" ht="28.5">
       <c r="A49" s="2" t="s">
@@ -3120,7 +3185,9 @@
       <c r="E49" s="3">
         <v>1</v>
       </c>
-      <c r="F49" s="3"/>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" ht="28.5">
       <c r="A50" s="2" t="s">
@@ -3132,7 +3199,9 @@
       <c r="E50" s="3">
         <v>1</v>
       </c>
-      <c r="F50" s="3"/>
+      <c r="F50" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" ht="28.5">
       <c r="A51" s="2" t="s">
@@ -3144,7 +3213,9 @@
       <c r="E51" s="3">
         <v>1</v>
       </c>
-      <c r="F51" s="3"/>
+      <c r="F51" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" ht="42.75">
       <c r="A52" s="2" t="s">
@@ -3159,7 +3230,9 @@
       <c r="E52" s="3">
         <v>1</v>
       </c>
-      <c r="F52" s="3"/>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" ht="42.75">
       <c r="A53" s="2" t="s">
@@ -3174,7 +3247,9 @@
       <c r="E53" s="3">
         <v>1</v>
       </c>
-      <c r="F53" s="3"/>
+      <c r="F53" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" ht="42.75">
       <c r="A54" s="2" t="s">
@@ -3189,7 +3264,9 @@
       <c r="E54" s="3">
         <v>1</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" ht="28.5">
       <c r="A55" s="2" t="s">
@@ -3201,7 +3278,9 @@
       <c r="E55" s="3">
         <v>1</v>
       </c>
-      <c r="F55" s="3"/>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" ht="28.5">
       <c r="A56" s="2" t="s">
@@ -3213,7 +3292,9 @@
       <c r="E56" s="3">
         <v>1</v>
       </c>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" ht="28.5">
       <c r="A57" s="2" t="s">
@@ -3225,7 +3306,9 @@
       <c r="E57" s="3">
         <v>1</v>
       </c>
-      <c r="F57" s="3"/>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" ht="42.75">
       <c r="A58" s="2" t="s">
@@ -3243,7 +3326,9 @@
       <c r="E58" s="3">
         <v>1</v>
       </c>
-      <c r="F58" s="3"/>
+      <c r="F58" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" ht="42.75">
       <c r="A59" s="2" t="s">
@@ -3261,7 +3346,9 @@
       <c r="E59" s="3">
         <v>1</v>
       </c>
-      <c r="F59" s="3"/>
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" ht="28.5">
       <c r="A60" s="2" t="s">
@@ -3276,7 +3363,9 @@
       <c r="E60" s="3">
         <v>1</v>
       </c>
-      <c r="F60" s="3"/>
+      <c r="F60" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" ht="28.5">
       <c r="A61" s="2" t="s">
@@ -3291,7 +3380,9 @@
       <c r="E61" s="3">
         <v>1</v>
       </c>
-      <c r="F61" s="3"/>
+      <c r="F61" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" ht="171">
       <c r="A62" s="2" t="s">
@@ -3307,7 +3398,9 @@
       <c r="E62" s="3">
         <v>12</v>
       </c>
-      <c r="F62" s="3"/>
+      <c r="F62" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="63" ht="28.5">
       <c r="A63" s="17" t="s">
@@ -3323,7 +3416,9 @@
         <v>120</v>
       </c>
       <c r="E63" s="19"/>
-      <c r="F63" s="3"/>
+      <c r="F63" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" ht="28.5">
       <c r="A64" s="17" t="s">
@@ -3337,7 +3432,9 @@
       </c>
       <c r="D64" s="18"/>
       <c r="E64" s="19"/>
-      <c r="F64" s="3"/>
+      <c r="F64" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" s="17" t="s">
@@ -3351,7 +3448,9 @@
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="19"/>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="17" t="s">
@@ -3365,7 +3464,9 @@
       </c>
       <c r="D66" s="18"/>
       <c r="E66" s="19"/>
-      <c r="F66" s="3"/>
+      <c r="F66" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" ht="14.25">
       <c r="A67" s="17" t="s">
@@ -3379,7 +3480,9 @@
       </c>
       <c r="D67" s="18"/>
       <c r="E67" s="19"/>
-      <c r="F67" s="3"/>
+      <c r="F67" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" ht="14.25">
       <c r="A68" s="17" t="s">
@@ -3393,7 +3496,9 @@
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="19"/>
-      <c r="F68" s="3"/>
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" ht="14.25">
       <c r="A69" s="17" t="s">
@@ -3407,7 +3512,9 @@
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="19"/>
-      <c r="F69" s="3"/>
+      <c r="F69" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" ht="14.25">
       <c r="A70" s="2" t="s">
@@ -3425,7 +3532,9 @@
       <c r="E70" s="3">
         <v>6</v>
       </c>
-      <c r="F70" s="3"/>
+      <c r="F70" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" s="2" t="s">
@@ -3439,7 +3548,9 @@
       <c r="E71" s="3">
         <v>1</v>
       </c>
-      <c r="F71" s="3"/>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="2" t="s">
@@ -3452,7 +3563,9 @@
       <c r="E72" s="3">
         <v>1</v>
       </c>
-      <c r="F72" s="3"/>
+      <c r="F72" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="2" t="s">
@@ -3465,7 +3578,9 @@
       <c r="E73" s="3">
         <v>1</v>
       </c>
-      <c r="F73" s="3"/>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" ht="14.25">
       <c r="A74" s="2" t="s">
@@ -3481,7 +3596,9 @@
       <c r="E74" s="3">
         <v>5</v>
       </c>
-      <c r="F74" s="3"/>
+      <c r="F74" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="75" ht="14.25">
       <c r="A75" s="2" t="s">
@@ -3499,7 +3616,9 @@
       <c r="E75" s="3">
         <v>5</v>
       </c>
-      <c r="F75" s="3"/>
+      <c r="F75" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="76" ht="14.25">
       <c r="A76" s="2" t="s">
@@ -3508,16 +3627,18 @@
       <c r="B76" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="7" t="s">
         <v>142</v>
       </c>
       <c r="E76" s="3">
         <v>11</v>
       </c>
-      <c r="F76" s="3"/>
+      <c r="F76" s="3">
+        <v>11</v>
+      </c>
     </row>
     <row r="77" ht="14.25">
       <c r="A77" s="17" t="s">
@@ -3531,7 +3652,9 @@
         <v>144</v>
       </c>
       <c r="E77" s="19"/>
-      <c r="F77" s="3"/>
+      <c r="F77" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" ht="14.25">
       <c r="A78" s="17" t="s">
@@ -3543,7 +3666,9 @@
       <c r="C78" s="21"/>
       <c r="D78" s="18"/>
       <c r="E78" s="19"/>
-      <c r="F78" s="3"/>
+      <c r="F78" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" ht="14.25">
       <c r="A79" s="17" t="s">
@@ -3555,7 +3680,9 @@
       <c r="C79" s="21"/>
       <c r="D79" s="18"/>
       <c r="E79" s="19"/>
-      <c r="F79" s="3"/>
+      <c r="F79" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" ht="14.25">
       <c r="A80" s="17" t="s">
@@ -3569,7 +3696,9 @@
       </c>
       <c r="D80" s="18"/>
       <c r="E80" s="19"/>
-      <c r="F80" s="3"/>
+      <c r="F80" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" ht="14.25">
       <c r="A81" s="17" t="s">
@@ -3583,7 +3712,9 @@
       </c>
       <c r="D81" s="18"/>
       <c r="E81" s="19"/>
-      <c r="F81" s="3"/>
+      <c r="F81" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" ht="14.25">
       <c r="A82" s="2" t="s">
@@ -3598,7 +3729,9 @@
       <c r="E82" s="3">
         <v>1</v>
       </c>
-      <c r="F82" s="3"/>
+      <c r="F82" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="83" ht="14.25">
       <c r="A83" s="2" t="s">
@@ -3616,7 +3749,9 @@
       <c r="E83" s="3">
         <v>1</v>
       </c>
-      <c r="F83" s="3"/>
+      <c r="F83" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" ht="14.25">
       <c r="A84" s="2" t="s">
@@ -3631,7 +3766,9 @@
       <c r="E84" s="3">
         <v>1</v>
       </c>
-      <c r="F84" s="3"/>
+      <c r="F84" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="85" ht="14.25">
       <c r="A85" s="2" t="s">
@@ -3649,7 +3786,9 @@
       <c r="E85" s="3">
         <v>1</v>
       </c>
-      <c r="F85" s="3"/>
+      <c r="F85" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="2" t="s">
@@ -3664,7 +3803,9 @@
       <c r="E86" s="3">
         <v>1</v>
       </c>
-      <c r="F86" s="3"/>
+      <c r="F86" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="2" t="s">
@@ -3676,7 +3817,9 @@
       <c r="E87" s="3">
         <v>1</v>
       </c>
-      <c r="F87" s="3"/>
+      <c r="F87" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" ht="14.25">
       <c r="A88" s="2" t="s">
@@ -3688,19 +3831,23 @@
       <c r="E88" s="3">
         <v>1</v>
       </c>
-      <c r="F88" s="3"/>
+      <c r="F88" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" ht="14.25">
       <c r="A89" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="7" t="s">
         <v>160</v>
       </c>
       <c r="E89" s="3">
         <v>1</v>
       </c>
-      <c r="F89" s="3"/>
+      <c r="F89" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="90" ht="14.25">
       <c r="A90" s="2" t="s">
@@ -3715,7 +3862,9 @@
       <c r="E90" s="3">
         <v>1</v>
       </c>
-      <c r="F90" s="3"/>
+      <c r="F90" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" ht="14.25">
       <c r="A91" s="2" t="s">
@@ -3727,7 +3876,9 @@
       <c r="E91" s="3">
         <v>1</v>
       </c>
-      <c r="F91" s="3"/>
+      <c r="F91" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="2" t="s">
@@ -3745,7 +3896,9 @@
       <c r="E92" s="3">
         <v>1</v>
       </c>
-      <c r="F92" s="3"/>
+      <c r="F92" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" ht="14.25">
       <c r="A93" s="2" t="s">
@@ -3760,13 +3913,15 @@
       <c r="E93" s="3">
         <v>1</v>
       </c>
-      <c r="F93" s="3"/>
+      <c r="F93" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="94" ht="14.25">
       <c r="A94" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="7" t="s">
         <v>166</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -3775,7 +3930,9 @@
       <c r="E94" s="3">
         <v>1</v>
       </c>
-      <c r="F94" s="3"/>
+      <c r="F94" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="95" ht="14.25">
       <c r="A95" s="2" t="s">
@@ -3790,7 +3947,9 @@
       <c r="E95" s="3">
         <v>1</v>
       </c>
-      <c r="F95" s="3"/>
+      <c r="F95" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="96" ht="14.25">
       <c r="A96" s="2" t="s">
@@ -3805,7 +3964,9 @@
       <c r="E96" s="3">
         <v>1</v>
       </c>
-      <c r="F96" s="3"/>
+      <c r="F96" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="97" ht="14.25">
       <c r="A97" s="2" t="s">
@@ -3818,7 +3979,9 @@
       <c r="E97" s="3">
         <v>1</v>
       </c>
-      <c r="F97" s="3"/>
+      <c r="F97" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="98" ht="14.25">
       <c r="A98" s="2" t="s">
@@ -3834,7 +3997,9 @@
       <c r="E98" s="3">
         <v>1</v>
       </c>
-      <c r="F98" s="3"/>
+      <c r="F98" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="99" ht="14.25">
       <c r="A99" s="2" t="s">
@@ -3847,7 +4012,9 @@
       <c r="E99" s="3">
         <v>1</v>
       </c>
-      <c r="F99" s="3"/>
+      <c r="F99" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" ht="14.25">
       <c r="A100" s="2" t="s">
@@ -3860,7 +4027,9 @@
       <c r="E100" s="3">
         <v>1</v>
       </c>
-      <c r="F100" s="3"/>
+      <c r="F100" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="101" ht="14.25">
       <c r="A101" s="2" t="s">
@@ -3876,7 +4045,9 @@
       <c r="E101" s="3">
         <v>1</v>
       </c>
-      <c r="F101" s="3"/>
+      <c r="F101" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" ht="14.25">
       <c r="A102" s="2" t="s">
@@ -3889,7 +4060,9 @@
       <c r="E102" s="3">
         <v>1</v>
       </c>
-      <c r="F102" s="3"/>
+      <c r="F102" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" ht="14.25">
       <c r="A103" s="2" t="s">
@@ -3907,7 +4080,9 @@
       <c r="E103" s="3">
         <v>1</v>
       </c>
-      <c r="F103" s="3"/>
+      <c r="F103" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="2" t="s">
@@ -3922,7 +4097,9 @@
       <c r="E104" s="3">
         <v>1</v>
       </c>
-      <c r="F104" s="3"/>
+      <c r="F104" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" ht="14.25">
       <c r="A105" s="2" t="s">
@@ -3940,7 +4117,9 @@
       <c r="E105" s="3">
         <v>1</v>
       </c>
-      <c r="F105" s="3"/>
+      <c r="F105" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="106" ht="14.25">
       <c r="A106" s="2" t="s">
@@ -3955,7 +4134,9 @@
       <c r="E106" s="3">
         <v>1</v>
       </c>
-      <c r="F106" s="3"/>
+      <c r="F106" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="107" ht="14.25">
       <c r="A107" s="2" t="s">
@@ -3973,7 +4154,9 @@
       <c r="E107" s="3">
         <v>1</v>
       </c>
-      <c r="F107" s="3"/>
+      <c r="F107" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="2" t="s">
@@ -3991,7 +4174,9 @@
       <c r="E108" s="3">
         <v>1</v>
       </c>
-      <c r="F108" s="3"/>
+      <c r="F108" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="2" t="s">
@@ -4005,7 +4190,9 @@
       <c r="E109" s="3">
         <v>1</v>
       </c>
-      <c r="F109" s="3"/>
+      <c r="F109" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="2" t="s">
@@ -4019,7 +4206,9 @@
       <c r="E110" s="3">
         <v>1</v>
       </c>
-      <c r="F110" s="3"/>
+      <c r="F110" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="111" ht="14.25">
       <c r="A111" s="2" t="s">
@@ -4033,7 +4222,9 @@
       <c r="E111" s="3">
         <v>1</v>
       </c>
-      <c r="F111" s="3"/>
+      <c r="F111" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="2" t="s">
@@ -4047,7 +4238,9 @@
       <c r="E112" s="3">
         <v>1</v>
       </c>
-      <c r="F112" s="3"/>
+      <c r="F112" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="113" ht="14.25">
       <c r="A113" s="2" t="s">
@@ -4063,7 +4256,9 @@
       <c r="E113" s="3">
         <v>1</v>
       </c>
-      <c r="F113" s="3"/>
+      <c r="F113" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="2" t="s">
@@ -4077,7 +4272,9 @@
       <c r="E114" s="3">
         <v>1</v>
       </c>
-      <c r="F114" s="3"/>
+      <c r="F114" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="2" t="s">
@@ -4095,7 +4292,9 @@
       <c r="E115" s="3">
         <v>1</v>
       </c>
-      <c r="F115" s="3"/>
+      <c r="F115" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="2" t="s">
@@ -4111,7 +4310,9 @@
       <c r="E116" s="3">
         <v>1</v>
       </c>
-      <c r="F116" s="3"/>
+      <c r="F116" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="2" t="s">
@@ -4125,7 +4326,9 @@
       <c r="E117" s="3">
         <v>1</v>
       </c>
-      <c r="F117" s="3"/>
+      <c r="F117" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="2" t="s">
@@ -4141,7 +4344,9 @@
       <c r="E118" s="3">
         <v>1</v>
       </c>
-      <c r="F118" s="3"/>
+      <c r="F118" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="2" t="s">
@@ -4155,7 +4360,9 @@
       <c r="E119" s="3">
         <v>1</v>
       </c>
-      <c r="F119" s="3"/>
+      <c r="F119" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="2" t="s">
@@ -4173,7 +4380,9 @@
       <c r="E120" s="3">
         <v>1</v>
       </c>
-      <c r="F120" s="3"/>
+      <c r="F120" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="2" t="s">
@@ -4189,7 +4398,9 @@
       <c r="E121" s="3">
         <v>1</v>
       </c>
-      <c r="F121" s="3"/>
+      <c r="F121" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="2" t="s">
@@ -4203,7 +4414,9 @@
       <c r="E122" s="3">
         <v>1</v>
       </c>
-      <c r="F122" s="3"/>
+      <c r="F122" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="123" ht="14.25">
       <c r="A123" s="2" t="s">
@@ -4219,7 +4432,9 @@
       <c r="E123" s="3">
         <v>1</v>
       </c>
-      <c r="F123" s="3"/>
+      <c r="F123" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" ht="14.25">
       <c r="A124" s="2" t="s">
@@ -4233,7 +4448,9 @@
       <c r="E124" s="3">
         <v>1</v>
       </c>
-      <c r="F124" s="3"/>
+      <c r="F124" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="125" ht="14.25">
       <c r="A125" s="2" t="s">
@@ -4251,7 +4468,9 @@
       <c r="E125" s="3">
         <v>1</v>
       </c>
-      <c r="F125" s="3"/>
+      <c r="F125" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="126" ht="14.25">
       <c r="A126" s="2" t="s">
@@ -4267,7 +4486,9 @@
       <c r="E126" s="3">
         <v>1</v>
       </c>
-      <c r="F126" s="3"/>
+      <c r="F126" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" ht="14.25">
       <c r="A127" s="2" t="s">
@@ -4281,7 +4502,9 @@
       <c r="E127" s="3">
         <v>1</v>
       </c>
-      <c r="F127" s="3"/>
+      <c r="F127" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="128" ht="14.25">
       <c r="A128" s="2" t="s">
@@ -4297,7 +4520,9 @@
       <c r="E128" s="3">
         <v>1</v>
       </c>
-      <c r="F128" s="3"/>
+      <c r="F128" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="129" ht="14.25">
       <c r="A129" s="2" t="s">
@@ -4311,7 +4536,9 @@
       <c r="E129" s="3">
         <v>1</v>
       </c>
-      <c r="F129" s="3"/>
+      <c r="F129" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="130" ht="14.25">
       <c r="A130" s="2" t="s">
@@ -4329,7 +4556,9 @@
       <c r="E130" s="3">
         <v>1</v>
       </c>
-      <c r="F130" s="3"/>
+      <c r="F130" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="131" ht="14.25">
       <c r="A131" s="2" t="s">
@@ -4345,7 +4574,9 @@
       <c r="E131" s="3">
         <v>1</v>
       </c>
-      <c r="F131" s="3"/>
+      <c r="F131" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="132" ht="14.25">
       <c r="A132" s="2" t="s">
@@ -4360,7 +4591,9 @@
       <c r="E132" s="3">
         <v>1</v>
       </c>
-      <c r="F132" s="3"/>
+      <c r="F132" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" ht="14.25">
       <c r="A133" s="2" t="s">
@@ -4375,7 +4608,9 @@
       <c r="E133" s="3">
         <v>1</v>
       </c>
-      <c r="F133" s="3"/>
+      <c r="F133" s="30">
+        <v>0</v>
+      </c>
     </row>
     <row r="134" ht="14.25">
       <c r="A134" s="2" t="s">
@@ -4390,7 +4625,9 @@
       <c r="E134" s="3">
         <v>1</v>
       </c>
-      <c r="F134" s="3"/>
+      <c r="F134" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" ht="14.25">
       <c r="A135" s="2" t="s">
@@ -4405,7 +4642,9 @@
       <c r="E135" s="3">
         <v>1</v>
       </c>
-      <c r="F135" s="3"/>
+      <c r="F135" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" ht="14.25">
       <c r="A136" s="2" t="s">
@@ -4420,7 +4659,9 @@
       <c r="E136" s="3">
         <v>1</v>
       </c>
-      <c r="F136" s="3"/>
+      <c r="F136" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="137" ht="14.25">
       <c r="A137" s="2" t="s">
@@ -4438,7 +4679,9 @@
       <c r="E137" s="3">
         <v>1</v>
       </c>
-      <c r="F137" s="3"/>
+      <c r="F137" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="138" ht="14.25">
       <c r="A138" s="2" t="s">
@@ -4450,13 +4693,15 @@
       <c r="E138" s="3">
         <v>1</v>
       </c>
-      <c r="F138" s="3"/>
+      <c r="F138" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" ht="14.25">
       <c r="A139" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B139" s="11" t="s">
+      <c r="B139" s="2" t="s">
         <v>224</v>
       </c>
       <c r="C139" s="1"/>
@@ -4464,109 +4709,112 @@
       <c r="E139" s="3">
         <v>1</v>
       </c>
-      <c r="F139" s="3"/>
+      <c r="F139" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="140" ht="14.25">
       <c r="A140" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B140" s="11" t="s">
+      <c r="B140" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C140" s="30" t="s">
+      <c r="C140" s="31" t="s">
         <v>226</v>
       </c>
       <c r="E140" s="3">
         <v>1</v>
       </c>
-      <c r="F140" s="3"/>
+      <c r="F140" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="141" ht="14.25">
       <c r="A141" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B141" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="C141" s="31" t="s">
-        <v>221</v>
-      </c>
+      <c r="B141" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C141" s="1"/>
       <c r="E141" s="3">
         <v>1</v>
       </c>
-      <c r="F141" s="3"/>
+      <c r="F141" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="142" ht="14.25">
       <c r="A142" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B142" s="11" t="s">
-        <v>56</v>
+      <c r="B142" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E142" s="3">
         <v>1</v>
       </c>
-      <c r="F142" s="3"/>
+      <c r="F142" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="143" ht="14.25">
       <c r="A143" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B143" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="D143" s="2" t="s">
-        <v>57</v>
+      <c r="B143" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E143" s="3">
         <v>1</v>
       </c>
-      <c r="F143" s="3"/>
+      <c r="F143" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="144" ht="14.25">
       <c r="A144" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B144" s="11" t="s">
-        <v>43</v>
+      <c r="B144" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C144" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E144" s="3">
         <v>1</v>
       </c>
-      <c r="F144" s="3"/>
+      <c r="F144" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="145" ht="14.25">
       <c r="A145" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B145" s="11" t="s">
-        <v>56</v>
+      <c r="B145" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C145" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D145" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E145" s="3">
         <v>1</v>
       </c>
-      <c r="F145" s="3"/>
+      <c r="F145" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="146" ht="14.25">
-      <c r="A146" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B146" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C146" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E146" s="3">
-        <v>1</v>
-      </c>
-      <c r="F146" s="3"/>
+      <c r="E146" s="3"/>
     </row>
     <row r="147" ht="14.25">
       <c r="E147" s="3"/>
@@ -6066,10 +6314,7 @@
       <c r="E645" s="3"/>
     </row>
     <row r="646" ht="14.25">
-      <c r="E646" s="3"/>
-    </row>
-    <row r="647" ht="14.25">
-      <c r="B647" s="2"/>
+      <c r="B646" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6097,10 +6342,10 @@
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="44.82421875"/>
     <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="44.19140625"/>
-    <col customWidth="1" min="3" max="3" style="31" width="68.28125"/>
-    <col customWidth="1" min="4" max="4" style="30" width="31.57421875"/>
-    <col bestFit="1" min="5" max="5" style="31" width="7.32421875"/>
-    <col min="6" max="16384" style="31" width="9.140625"/>
+    <col customWidth="1" min="3" max="3" style="32" width="68.28125"/>
+    <col customWidth="1" min="4" max="4" style="31" width="31.57421875"/>
+    <col bestFit="1" min="5" max="5" style="32" width="7.32421875"/>
+    <col min="6" max="16384" style="32" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.5">
@@ -6108,7 +6353,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -6119,124 +6364,140 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="31"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31">
-        <v>1</v>
-      </c>
-      <c r="F2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32">
+        <v>1</v>
+      </c>
+      <c r="F2" s="32">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" ht="28.5">
       <c r="A3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31">
-        <v>1</v>
-      </c>
-      <c r="F3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32">
+        <v>1</v>
+      </c>
+      <c r="F3" s="32">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B4" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="31">
-        <v>1</v>
-      </c>
-      <c r="F4" s="31"/>
+      <c r="E4" s="32">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" ht="57">
       <c r="A5" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="31">
-        <v>1</v>
-      </c>
-      <c r="F5" s="31"/>
+      <c r="E5" s="32">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B6" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="31">
-        <v>1</v>
-      </c>
-      <c r="F6" s="31"/>
+      <c r="E6" s="32">
+        <v>1</v>
+      </c>
+      <c r="F6" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B7" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="31">
-        <v>1</v>
-      </c>
-      <c r="F7" s="31"/>
+      <c r="E7" s="32">
+        <v>1</v>
+      </c>
+      <c r="F7" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" ht="57">
       <c r="A8" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B8" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="31">
-        <v>1</v>
-      </c>
-      <c r="F8" s="31"/>
+      <c r="E8" s="32">
+        <v>1</v>
+      </c>
+      <c r="F8" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B9" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="31">
-        <v>1</v>
-      </c>
-      <c r="F9" s="31"/>
+      <c r="E9" s="32">
+        <v>1</v>
+      </c>
+      <c r="F9" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" ht="57">
       <c r="A10" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B10" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -6245,33 +6506,37 @@
       <c r="D10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="31">
-        <v>1</v>
-      </c>
-      <c r="F10" s="31"/>
+      <c r="E10" s="32">
+        <v>1</v>
+      </c>
+      <c r="F10" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" ht="28.5">
       <c r="A11" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B11" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="31">
-        <v>1</v>
-      </c>
-      <c r="F11" s="31"/>
+      <c r="E11" s="32">
+        <v>1</v>
+      </c>
+      <c r="F11" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" ht="57">
       <c r="A12" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>249</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>60</v>
@@ -6279,356 +6544,398 @@
       <c r="D12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="31">
-        <v>1</v>
-      </c>
-      <c r="F12" s="31"/>
+      <c r="E12" s="32">
+        <v>1</v>
+      </c>
+      <c r="F12" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" ht="28.5">
       <c r="A13" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B13" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="31">
-        <v>1</v>
-      </c>
-      <c r="F13" s="31"/>
+      <c r="E13" s="32">
+        <v>1</v>
+      </c>
+      <c r="F13" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" ht="28.5">
       <c r="A14" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="B14" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="33" t="s">
+      <c r="D14" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="E14" s="31">
-        <v>1</v>
-      </c>
-      <c r="F14" s="31"/>
+      <c r="E14" s="32">
+        <v>1</v>
+      </c>
+      <c r="F14" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" ht="28.5">
       <c r="A15" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B15" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E15" s="31">
-        <v>1</v>
-      </c>
-      <c r="F15" s="31"/>
+      <c r="D15" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="E15" s="32">
+        <v>1</v>
+      </c>
+      <c r="F15" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" ht="85.5">
       <c r="A16" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E16" s="31">
-        <v>1</v>
-      </c>
-      <c r="F16" s="31"/>
+      <c r="E16" s="32">
+        <v>1</v>
+      </c>
+      <c r="F16" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" ht="28.5">
       <c r="A17" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B17" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E17" s="31">
-        <v>1</v>
-      </c>
-      <c r="F17" s="31"/>
+      <c r="D17" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" s="32">
+        <v>1</v>
+      </c>
+      <c r="F17" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" ht="85.5">
       <c r="A18" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B18" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="E18" s="31">
-        <v>1</v>
-      </c>
-      <c r="F18" s="31"/>
+      <c r="D18" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E18" s="32">
+        <v>1</v>
+      </c>
+      <c r="F18" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" ht="28.5">
       <c r="A19" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B19" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="E19" s="31">
-        <v>1</v>
-      </c>
-      <c r="F19" s="31"/>
+      <c r="D19" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="E19" s="32">
+        <v>1</v>
+      </c>
+      <c r="F19" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" ht="28.5">
       <c r="A20" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="D20" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="E20" s="31">
-        <v>1</v>
-      </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
+      <c r="E20" s="32">
+        <v>1</v>
+      </c>
+      <c r="F20" s="34">
+        <v>0</v>
+      </c>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" ht="28.5">
       <c r="A21" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B21" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="E21" s="31">
-        <v>1</v>
-      </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
+      <c r="D21" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E21" s="32">
+        <v>1</v>
+      </c>
+      <c r="F21" s="32">
+        <v>1</v>
+      </c>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" ht="85.5">
       <c r="A22" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B22" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E22" s="31">
-        <v>1</v>
-      </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="E22" s="32">
+        <v>1</v>
+      </c>
+      <c r="F22" s="32">
+        <v>1</v>
+      </c>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" ht="28.5">
       <c r="A23" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B23" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="E23" s="31">
-        <v>1</v>
-      </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
+      <c r="D23" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E23" s="32">
+        <v>1</v>
+      </c>
+      <c r="F23" s="32">
+        <v>1</v>
+      </c>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" ht="85.5">
       <c r="A24" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B24" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E24" s="31">
-        <v>1</v>
-      </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="D24" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E24" s="32">
+        <v>1</v>
+      </c>
+      <c r="F24" s="32">
+        <v>1</v>
+      </c>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" ht="28.5">
       <c r="A25" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B25" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="E25" s="31">
-        <v>1</v>
-      </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="D25" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E25" s="32">
+        <v>1</v>
+      </c>
+      <c r="F25" s="32">
+        <v>1</v>
+      </c>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" ht="28.5">
       <c r="A26" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C26" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="D26" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="C26" s="31" t="s">
-        <v>270</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="E26" s="31">
-        <v>1</v>
-      </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
+      <c r="E26" s="32">
+        <v>1</v>
+      </c>
+      <c r="F26" s="32">
+        <v>0</v>
+      </c>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" ht="28.5">
       <c r="A27" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="35" t="s">
         <v>271</v>
       </c>
-      <c r="B27" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>272</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="E27" s="31">
-        <v>1</v>
-      </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
+      <c r="D27" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E27" s="32">
+        <v>1</v>
+      </c>
+      <c r="F27" s="32">
+        <v>1</v>
+      </c>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" ht="85.5">
       <c r="A28" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B28" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C28" s="35"/>
-      <c r="D28" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E28" s="31">
-        <v>1</v>
-      </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
+      <c r="D28" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E28" s="32">
+        <v>1</v>
+      </c>
+      <c r="F28" s="32">
+        <v>1</v>
+      </c>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" ht="28.5">
       <c r="A29" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E29" s="32">
+        <v>1</v>
+      </c>
+      <c r="F29" s="32">
+        <v>1</v>
+      </c>
+      <c r="G29" s="32"/>
+    </row>
+    <row r="30" ht="85.5">
+      <c r="A30" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B29" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="E29" s="31">
-        <v>1</v>
-      </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-    </row>
-    <row r="30" ht="85.5">
-      <c r="A30" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E30" s="31">
-        <v>1</v>
-      </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
+      <c r="D30" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E30" s="32">
+        <v>1</v>
+      </c>
+      <c r="F30" s="32">
+        <v>1</v>
+      </c>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" ht="28.5">
-      <c r="A31" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="B31" s="32" t="s">
+      <c r="A31" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="E31" s="31">
-        <v>1</v>
-      </c>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
+      <c r="D31" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E31" s="32">
+        <v>1</v>
+      </c>
+      <c r="F31" s="32">
+        <v>1</v>
+      </c>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E32" s="37">
         <v>1</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
+      <c r="F32" s="34">
+        <v>0</v>
+      </c>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>33</v>
@@ -6637,27 +6944,31 @@
       <c r="E33" s="37">
         <v>1</v>
       </c>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
+      <c r="F33" s="32">
+        <v>0</v>
+      </c>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="35"/>
-      <c r="D34" s="30"/>
+      <c r="D34" s="31"/>
       <c r="E34" s="37">
         <v>1</v>
       </c>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
+      <c r="F34" s="32">
+        <v>0</v>
+      </c>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" ht="14.25">
       <c r="A35" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>33</v>
@@ -6665,41 +6976,47 @@
       <c r="E35" s="37">
         <v>1</v>
       </c>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
+      <c r="F35" s="32">
+        <v>0</v>
+      </c>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="30"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="37">
         <v>1</v>
       </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
+      <c r="F36" s="32">
+        <v>0</v>
+      </c>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="31"/>
+      <c r="C37" s="32"/>
       <c r="E37" s="37">
         <v>1</v>
       </c>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
+      <c r="F37" s="32">
+        <v>0</v>
+      </c>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>33</v>
@@ -6710,12 +7027,14 @@
       <c r="E38" s="37">
         <v>1</v>
       </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
+      <c r="F38" s="32">
+        <v>0</v>
+      </c>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>33</v>
@@ -6726,30 +7045,32 @@
       <c r="E39" s="37">
         <v>1</v>
       </c>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
+      <c r="F39" s="32">
+        <v>0</v>
+      </c>
+      <c r="G39" s="32"/>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="31"/>
-      <c r="E40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
-      <c r="E41" s="31"/>
+      <c r="E41" s="32"/>
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
-      <c r="E42" s="31"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="31"/>
-      <c r="E43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="E43" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Finished tutorial on tidy models. Implemented better imputation of missing values for CBP. Collected homicide data from CDC.
</commit_message>
<xml_diff>
--- a/Variable List.xlsx
+++ b/Variable List.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
   <si>
     <t>Variable</t>
   </si>
@@ -1567,6 +1568,15 @@
   </si>
   <si>
     <t xml:space="preserve">Ratio of female to male LFPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCR Crime data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDC Homicide data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population density</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1723,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="34">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1732,13 +1742,6 @@
     </xf>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1805,16 +1808,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2362,7 +2361,7 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1"/>
@@ -2377,7 +2376,7 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2394,7 +2393,7 @@
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2411,7 +2410,7 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2428,7 +2427,7 @@
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2445,7 +2444,7 @@
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2465,7 +2464,7 @@
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -2485,7 +2484,7 @@
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -2505,7 +2504,7 @@
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
@@ -2520,37 +2519,37 @@
       </c>
     </row>
     <row r="11" ht="28.5">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="12"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="12"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="12"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="3">
         <v>0</v>
       </c>
@@ -2559,7 +2558,7 @@
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="3">
@@ -2591,7 +2590,7 @@
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="3">
@@ -2668,7 +2667,7 @@
       <c r="C20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="3">
@@ -2679,17 +2678,17 @@
       </c>
     </row>
     <row r="21" ht="28.5">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="14" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="10">
         <v>1</v>
       </c>
       <c r="F21" s="3">
@@ -2751,7 +2750,7 @@
       <c r="B25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -2771,7 +2770,7 @@
       <c r="B26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D26" s="2"/>
@@ -2835,7 +2834,7 @@
       <c r="B30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -2855,7 +2854,7 @@
       <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E31" s="3">
@@ -2923,7 +2922,7 @@
       <c r="B35" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -2943,7 +2942,7 @@
       <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -3094,7 +3093,7 @@
       <c r="B44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -3114,7 +3113,7 @@
       <c r="B45" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E45" s="3">
@@ -3317,7 +3316,7 @@
       <c r="B58" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -3337,7 +3336,7 @@
       <c r="B59" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -3357,7 +3356,7 @@
       <c r="B60" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C60" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E60" s="3">
@@ -3374,7 +3373,7 @@
       <c r="B61" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E61" s="3">
@@ -3391,7 +3390,7 @@
       <c r="B62" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="14" t="s">
         <v>116</v>
       </c>
       <c r="D62" s="2"/>
@@ -3403,115 +3402,115 @@
       </c>
     </row>
     <row r="63" ht="28.5">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C63" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D63" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E63" s="19"/>
+      <c r="E63" s="17"/>
       <c r="F63" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="64" ht="28.5">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C64" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D64" s="18"/>
-      <c r="E64" s="19"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="17"/>
       <c r="F64" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="65" ht="14.25">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C65" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="19"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="17"/>
       <c r="F65" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="66" ht="14.25">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D66" s="18"/>
-      <c r="E66" s="19"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="17"/>
       <c r="F66" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="67" ht="14.25">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D67" s="18"/>
-      <c r="E67" s="19"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="17"/>
       <c r="F67" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D68" s="18"/>
-      <c r="E68" s="19"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="17"/>
       <c r="F68" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="69" ht="14.25">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D69" s="18"/>
-      <c r="E69" s="19"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="17"/>
       <c r="F69" s="3">
         <v>0</v>
       </c>
@@ -3627,10 +3626,10 @@
       <c r="B76" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E76" s="3">
@@ -3641,77 +3640,77 @@
       </c>
     </row>
     <row r="77" ht="14.25">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C77" s="21"/>
-      <c r="D77" s="18" t="s">
+      <c r="C77" s="19"/>
+      <c r="D77" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E77" s="19"/>
+      <c r="E77" s="17"/>
       <c r="F77" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="78" ht="14.25">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C78" s="21"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="17"/>
       <c r="F78" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="79" ht="14.25">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C79" s="21"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="17"/>
       <c r="F79" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="80" ht="14.25">
-      <c r="A80" s="17" t="s">
+      <c r="A80" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C80" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D80" s="18"/>
-      <c r="E80" s="19"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="17"/>
       <c r="F80" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="81" ht="14.25">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C81" s="22" t="s">
+      <c r="C81" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D81" s="18"/>
-      <c r="E81" s="19"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="17"/>
       <c r="F81" s="3">
         <v>0</v>
       </c>
@@ -3777,7 +3776,7 @@
       <c r="B85" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C85" s="15" t="s">
+      <c r="C85" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3797,7 +3796,7 @@
       <c r="B86" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E86" s="3">
@@ -3839,7 +3838,7 @@
       <c r="A89" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E89" s="3">
@@ -3887,7 +3886,7 @@
       <c r="B92" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="C92" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D92" s="2" t="s">
@@ -3907,7 +3906,7 @@
       <c r="B93" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="C93" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E93" s="3">
@@ -3921,7 +3920,7 @@
       <c r="A94" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B94" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -4071,7 +4070,7 @@
       <c r="B103" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C103" s="15" t="s">
+      <c r="C103" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -4091,7 +4090,7 @@
       <c r="B104" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C104" s="15" t="s">
+      <c r="C104" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E104" s="3">
@@ -4108,7 +4107,7 @@
       <c r="B105" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C105" s="15" t="s">
+      <c r="C105" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -4128,7 +4127,7 @@
       <c r="B106" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C106" s="15" t="s">
+      <c r="C106" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E106" s="3">
@@ -4145,7 +4144,7 @@
       <c r="B107" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="15" t="s">
+      <c r="C107" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -4165,10 +4164,10 @@
       <c r="B108" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C108" s="23" t="s">
+      <c r="C108" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="D108" s="24" t="s">
+      <c r="D108" s="22" t="s">
         <v>186</v>
       </c>
       <c r="E108" s="3">
@@ -4185,8 +4184,8 @@
       <c r="B109" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C109" s="25"/>
-      <c r="D109" s="24"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="22"/>
       <c r="E109" s="3">
         <v>1</v>
       </c>
@@ -4201,8 +4200,8 @@
       <c r="B110" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C110" s="25"/>
-      <c r="D110" s="24"/>
+      <c r="C110" s="23"/>
+      <c r="D110" s="22"/>
       <c r="E110" s="3">
         <v>1</v>
       </c>
@@ -4217,8 +4216,8 @@
       <c r="B111" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C111" s="26"/>
-      <c r="D111" s="24"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="22"/>
       <c r="E111" s="3">
         <v>1</v>
       </c>
@@ -4233,8 +4232,8 @@
       <c r="B112" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C112" s="27"/>
-      <c r="D112" s="28"/>
+      <c r="C112" s="25"/>
+      <c r="D112" s="26"/>
       <c r="E112" s="3">
         <v>1</v>
       </c>
@@ -4249,7 +4248,7 @@
       <c r="B113" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C113" s="27"/>
+      <c r="C113" s="25"/>
       <c r="D113" s="2" t="s">
         <v>57</v>
       </c>
@@ -4267,7 +4266,7 @@
       <c r="B114" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C114" s="27"/>
+      <c r="C114" s="25"/>
       <c r="D114" s="2"/>
       <c r="E114" s="3">
         <v>1</v>
@@ -4283,7 +4282,7 @@
       <c r="B115" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C115" s="15" t="s">
+      <c r="C115" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -4303,7 +4302,7 @@
       <c r="B116" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C116" s="15" t="s">
+      <c r="C116" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D116" s="2"/>
@@ -4321,7 +4320,7 @@
       <c r="B117" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C117" s="27"/>
+      <c r="C117" s="25"/>
       <c r="D117" s="2"/>
       <c r="E117" s="3">
         <v>1</v>
@@ -4337,7 +4336,7 @@
       <c r="B118" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="27"/>
+      <c r="C118" s="25"/>
       <c r="D118" s="2" t="s">
         <v>57</v>
       </c>
@@ -4355,7 +4354,7 @@
       <c r="B119" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C119" s="27"/>
+      <c r="C119" s="25"/>
       <c r="D119" s="2"/>
       <c r="E119" s="3">
         <v>1</v>
@@ -4371,7 +4370,7 @@
       <c r="B120" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C120" s="15" t="s">
+      <c r="C120" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D120" s="2" t="s">
@@ -4391,7 +4390,7 @@
       <c r="B121" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C121" s="15" t="s">
+      <c r="C121" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D121" s="2"/>
@@ -4409,7 +4408,7 @@
       <c r="B122" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C122" s="27"/>
+      <c r="C122" s="25"/>
       <c r="D122" s="2"/>
       <c r="E122" s="3">
         <v>1</v>
@@ -4425,7 +4424,7 @@
       <c r="B123" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C123" s="27"/>
+      <c r="C123" s="25"/>
       <c r="D123" s="2" t="s">
         <v>57</v>
       </c>
@@ -4443,7 +4442,7 @@
       <c r="B124" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C124" s="27"/>
+      <c r="C124" s="25"/>
       <c r="D124" s="2"/>
       <c r="E124" s="3">
         <v>1</v>
@@ -4459,7 +4458,7 @@
       <c r="B125" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C125" s="15" t="s">
+      <c r="C125" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -4479,7 +4478,7 @@
       <c r="B126" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C126" s="15" t="s">
+      <c r="C126" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D126" s="2"/>
@@ -4497,7 +4496,7 @@
       <c r="B127" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C127" s="27"/>
+      <c r="C127" s="25"/>
       <c r="D127" s="2"/>
       <c r="E127" s="3">
         <v>1</v>
@@ -4513,7 +4512,7 @@
       <c r="B128" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C128" s="27"/>
+      <c r="C128" s="25"/>
       <c r="D128" s="2" t="s">
         <v>57</v>
       </c>
@@ -4531,7 +4530,7 @@
       <c r="B129" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C129" s="27"/>
+      <c r="C129" s="25"/>
       <c r="D129" s="2"/>
       <c r="E129" s="3">
         <v>1</v>
@@ -4547,7 +4546,7 @@
       <c r="B130" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C130" s="15" t="s">
+      <c r="C130" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D130" s="2" t="s">
@@ -4567,7 +4566,7 @@
       <c r="B131" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C131" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D131" s="2"/>
@@ -4585,7 +4584,7 @@
       <c r="B132" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C132" s="29" t="s">
+      <c r="C132" s="27" t="s">
         <v>212</v>
       </c>
       <c r="E132" s="3">
@@ -4602,13 +4601,13 @@
       <c r="B133" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C133" s="29" t="s">
+      <c r="C133" s="27" t="s">
         <v>214</v>
       </c>
       <c r="E133" s="3">
         <v>1</v>
       </c>
-      <c r="F133" s="30">
+      <c r="F133" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4619,7 +4618,7 @@
       <c r="B134" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C134" s="29" t="s">
+      <c r="C134" s="27" t="s">
         <v>216</v>
       </c>
       <c r="E134" s="3">
@@ -4636,7 +4635,7 @@
       <c r="B135" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C135" s="29" t="s">
+      <c r="C135" s="27" t="s">
         <v>212</v>
       </c>
       <c r="E135" s="3">
@@ -4653,7 +4652,7 @@
       <c r="B136" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C136" s="29" t="s">
+      <c r="C136" s="27" t="s">
         <v>219</v>
       </c>
       <c r="E136" s="3">
@@ -4720,7 +4719,7 @@
       <c r="B140" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C140" s="31" t="s">
+      <c r="C140" s="28" t="s">
         <v>226</v>
       </c>
       <c r="E140" s="3">
@@ -4783,7 +4782,7 @@
       <c r="B144" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C144" s="15" t="s">
+      <c r="C144" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D144" s="2" t="s">
@@ -4803,7 +4802,7 @@
       <c r="B145" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C145" s="15" t="s">
+      <c r="C145" s="13" t="s">
         <v>60</v>
       </c>
       <c r="E145" s="3">
@@ -6342,10 +6341,10 @@
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="44.82421875"/>
     <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="44.19140625"/>
-    <col customWidth="1" min="3" max="3" style="32" width="68.28125"/>
-    <col customWidth="1" min="4" max="4" style="31" width="31.57421875"/>
-    <col bestFit="1" min="5" max="5" style="32" width="7.32421875"/>
-    <col min="6" max="16384" style="32" width="9.140625"/>
+    <col customWidth="1" min="3" max="3" style="29" width="68.28125"/>
+    <col customWidth="1" min="4" max="4" style="28" width="31.57421875"/>
+    <col bestFit="1" min="5" max="5" style="29" width="7.32421875"/>
+    <col min="6" max="16384" style="29" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.5">
@@ -6364,7 +6363,7 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -6373,14 +6372,14 @@
       <c r="B2" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32">
-        <v>1</v>
-      </c>
-      <c r="F2" s="32">
+      <c r="D2" s="28"/>
+      <c r="E2" s="29">
+        <v>1</v>
+      </c>
+      <c r="F2" s="29">
         <v>0</v>
       </c>
     </row>
@@ -6394,11 +6393,11 @@
       <c r="C3" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32">
-        <v>1</v>
-      </c>
-      <c r="F3" s="32">
+      <c r="D3" s="28"/>
+      <c r="E3" s="29">
+        <v>1</v>
+      </c>
+      <c r="F3" s="29">
         <v>0</v>
       </c>
     </row>
@@ -6409,10 +6408,10 @@
       <c r="B4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="32">
-        <v>1</v>
-      </c>
-      <c r="F4" s="32">
+      <c r="E4" s="29">
+        <v>1</v>
+      </c>
+      <c r="F4" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6426,10 +6425,10 @@
       <c r="D5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="32">
-        <v>1</v>
-      </c>
-      <c r="F5" s="32">
+      <c r="E5" s="29">
+        <v>1</v>
+      </c>
+      <c r="F5" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6440,10 +6439,10 @@
       <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="32">
-        <v>1</v>
-      </c>
-      <c r="F6" s="32">
+      <c r="E6" s="29">
+        <v>1</v>
+      </c>
+      <c r="F6" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6454,10 +6453,10 @@
       <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="32">
-        <v>1</v>
-      </c>
-      <c r="F7" s="32">
+      <c r="E7" s="29">
+        <v>1</v>
+      </c>
+      <c r="F7" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6471,10 +6470,10 @@
       <c r="D8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="32">
-        <v>1</v>
-      </c>
-      <c r="F8" s="32">
+      <c r="E8" s="29">
+        <v>1</v>
+      </c>
+      <c r="F8" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6486,10 +6485,10 @@
         <v>56</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="32">
-        <v>1</v>
-      </c>
-      <c r="F9" s="32">
+      <c r="E9" s="29">
+        <v>1</v>
+      </c>
+      <c r="F9" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6500,16 +6499,16 @@
       <c r="B10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="32">
-        <v>1</v>
-      </c>
-      <c r="F10" s="32">
+      <c r="E10" s="29">
+        <v>1</v>
+      </c>
+      <c r="F10" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6520,14 +6519,14 @@
       <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="32">
-        <v>1</v>
-      </c>
-      <c r="F11" s="32">
+      <c r="E11" s="29">
+        <v>1</v>
+      </c>
+      <c r="F11" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6538,16 +6537,16 @@
       <c r="B12" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="32">
-        <v>1</v>
-      </c>
-      <c r="F12" s="32">
+      <c r="E12" s="29">
+        <v>1</v>
+      </c>
+      <c r="F12" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6558,13 +6557,13 @@
       <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="32">
-        <v>1</v>
-      </c>
-      <c r="F13" s="32">
+      <c r="E13" s="29">
+        <v>1</v>
+      </c>
+      <c r="F13" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6575,16 +6574,16 @@
       <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="32">
-        <v>1</v>
-      </c>
-      <c r="F14" s="32">
+      <c r="E14" s="29">
+        <v>1</v>
+      </c>
+      <c r="F14" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6595,13 +6594,13 @@
       <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="E15" s="32">
-        <v>1</v>
-      </c>
-      <c r="F15" s="32">
+      <c r="E15" s="29">
+        <v>1</v>
+      </c>
+      <c r="F15" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6615,10 +6614,10 @@
       <c r="D16" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E16" s="32">
-        <v>1</v>
-      </c>
-      <c r="F16" s="32">
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6629,13 +6628,13 @@
       <c r="B17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="E17" s="32">
-        <v>1</v>
-      </c>
-      <c r="F17" s="32">
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6646,16 +6645,16 @@
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E18" s="32">
-        <v>1</v>
-      </c>
-      <c r="F18" s="32">
+      <c r="E18" s="29">
+        <v>1</v>
+      </c>
+      <c r="F18" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6666,16 +6665,16 @@
       <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="E19" s="32">
-        <v>1</v>
-      </c>
-      <c r="F19" s="32">
+      <c r="E19" s="29">
+        <v>1</v>
+      </c>
+      <c r="F19" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6686,16 +6685,16 @@
       <c r="B20" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="E20" s="32">
-        <v>1</v>
-      </c>
-      <c r="F20" s="34">
+      <c r="E20" s="29">
+        <v>1</v>
+      </c>
+      <c r="F20" s="29">
         <v>0</v>
       </c>
-      <c r="G20" s="32"/>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" ht="28.5">
       <c r="A21" s="2" t="s">
@@ -6704,16 +6703,16 @@
       <c r="B21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="E21" s="32">
-        <v>1</v>
-      </c>
-      <c r="F21" s="32">
-        <v>1</v>
-      </c>
-      <c r="G21" s="32"/>
+      <c r="E21" s="29">
+        <v>1</v>
+      </c>
+      <c r="F21" s="29">
+        <v>1</v>
+      </c>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" ht="85.5">
       <c r="A22" s="2" t="s">
@@ -6725,13 +6724,13 @@
       <c r="D22" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E22" s="32">
-        <v>1</v>
-      </c>
-      <c r="F22" s="32">
-        <v>1</v>
-      </c>
-      <c r="G22" s="32"/>
+      <c r="E22" s="29">
+        <v>1</v>
+      </c>
+      <c r="F22" s="29">
+        <v>1</v>
+      </c>
+      <c r="G22" s="29"/>
     </row>
     <row r="23" ht="28.5">
       <c r="A23" s="2" t="s">
@@ -6740,16 +6739,16 @@
       <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="E23" s="32">
-        <v>1</v>
-      </c>
-      <c r="F23" s="32">
-        <v>1</v>
-      </c>
-      <c r="G23" s="32"/>
+      <c r="E23" s="29">
+        <v>1</v>
+      </c>
+      <c r="F23" s="29">
+        <v>1</v>
+      </c>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" ht="85.5">
       <c r="A24" s="2" t="s">
@@ -6758,19 +6757,19 @@
       <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E24" s="32">
-        <v>1</v>
-      </c>
-      <c r="F24" s="32">
-        <v>1</v>
-      </c>
-      <c r="G24" s="32"/>
+      <c r="E24" s="29">
+        <v>1</v>
+      </c>
+      <c r="F24" s="29">
+        <v>1</v>
+      </c>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" ht="28.5">
       <c r="A25" s="2" t="s">
@@ -6779,19 +6778,19 @@
       <c r="B25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="E25" s="32">
-        <v>1</v>
-      </c>
-      <c r="F25" s="32">
-        <v>1</v>
-      </c>
-      <c r="G25" s="32"/>
+      <c r="E25" s="29">
+        <v>1</v>
+      </c>
+      <c r="F25" s="29">
+        <v>1</v>
+      </c>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" ht="28.5">
       <c r="A26" s="2" t="s">
@@ -6800,19 +6799,19 @@
       <c r="B26" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="E26" s="32">
-        <v>1</v>
-      </c>
-      <c r="F26" s="32">
+      <c r="E26" s="29">
+        <v>1</v>
+      </c>
+      <c r="F26" s="29">
         <v>0</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="29"/>
     </row>
     <row r="27" ht="28.5">
       <c r="A27" s="2" t="s">
@@ -6821,19 +6820,19 @@
       <c r="B27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="E27" s="32">
-        <v>1</v>
-      </c>
-      <c r="F27" s="32">
-        <v>1</v>
-      </c>
-      <c r="G27" s="32"/>
+      <c r="E27" s="29">
+        <v>1</v>
+      </c>
+      <c r="F27" s="29">
+        <v>1</v>
+      </c>
+      <c r="G27" s="29"/>
     </row>
     <row r="28" ht="85.5">
       <c r="A28" s="2" t="s">
@@ -6842,17 +6841,17 @@
       <c r="B28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="35"/>
+      <c r="C28" s="31"/>
       <c r="D28" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E28" s="32">
-        <v>1</v>
-      </c>
-      <c r="F28" s="32">
-        <v>1</v>
-      </c>
-      <c r="G28" s="32"/>
+      <c r="E28" s="29">
+        <v>1</v>
+      </c>
+      <c r="F28" s="29">
+        <v>1</v>
+      </c>
+      <c r="G28" s="29"/>
     </row>
     <row r="29" ht="28.5">
       <c r="A29" s="2" t="s">
@@ -6861,17 +6860,17 @@
       <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="31" t="s">
+      <c r="C29" s="31"/>
+      <c r="D29" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="E29" s="32">
-        <v>1</v>
-      </c>
-      <c r="F29" s="32">
-        <v>1</v>
-      </c>
-      <c r="G29" s="32"/>
+      <c r="E29" s="29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="29"/>
     </row>
     <row r="30" ht="85.5">
       <c r="A30" s="2" t="s">
@@ -6880,19 +6879,19 @@
       <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E30" s="32">
-        <v>1</v>
-      </c>
-      <c r="F30" s="32">
-        <v>1</v>
-      </c>
-      <c r="G30" s="32"/>
+      <c r="E30" s="29">
+        <v>1</v>
+      </c>
+      <c r="F30" s="29">
+        <v>1</v>
+      </c>
+      <c r="G30" s="29"/>
     </row>
     <row r="31" ht="28.5">
       <c r="A31" s="2" t="s">
@@ -6901,19 +6900,19 @@
       <c r="B31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="E31" s="32">
-        <v>1</v>
-      </c>
-      <c r="F31" s="32">
-        <v>1</v>
-      </c>
-      <c r="G31" s="32"/>
+      <c r="E31" s="29">
+        <v>1</v>
+      </c>
+      <c r="F31" s="29">
+        <v>1</v>
+      </c>
+      <c r="G31" s="29"/>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="2" t="s">
@@ -6922,16 +6921,16 @@
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="32" t="s">
         <v>277</v>
       </c>
-      <c r="E32" s="37">
-        <v>1</v>
-      </c>
-      <c r="F32" s="34">
+      <c r="E32" s="33">
+        <v>1</v>
+      </c>
+      <c r="F32" s="29">
         <v>0</v>
       </c>
-      <c r="G32" s="32"/>
+      <c r="G32" s="29"/>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="2" t="s">
@@ -6940,14 +6939,14 @@
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="35"/>
-      <c r="E33" s="37">
-        <v>1</v>
-      </c>
-      <c r="F33" s="32">
+      <c r="C33" s="31"/>
+      <c r="E33" s="33">
+        <v>1</v>
+      </c>
+      <c r="F33" s="29">
         <v>0</v>
       </c>
-      <c r="G33" s="32"/>
+      <c r="G33" s="29"/>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="2" t="s">
@@ -6956,15 +6955,15 @@
       <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="37">
-        <v>1</v>
-      </c>
-      <c r="F34" s="32">
+      <c r="C34" s="31"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="33">
+        <v>1</v>
+      </c>
+      <c r="F34" s="29">
         <v>0</v>
       </c>
-      <c r="G34" s="32"/>
+      <c r="G34" s="29"/>
     </row>
     <row r="35" ht="14.25">
       <c r="A35" s="2" t="s">
@@ -6973,13 +6972,13 @@
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="37">
-        <v>1</v>
-      </c>
-      <c r="F35" s="32">
+      <c r="E35" s="33">
+        <v>1</v>
+      </c>
+      <c r="F35" s="29">
         <v>0</v>
       </c>
-      <c r="G35" s="32"/>
+      <c r="G35" s="29"/>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="2" t="s">
@@ -6988,15 +6987,15 @@
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="37">
-        <v>1</v>
-      </c>
-      <c r="F36" s="32">
+      <c r="C36" s="29"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="33">
+        <v>1</v>
+      </c>
+      <c r="F36" s="29">
         <v>0</v>
       </c>
-      <c r="G36" s="32"/>
+      <c r="G36" s="29"/>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="2" t="s">
@@ -7005,14 +7004,14 @@
       <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="E37" s="37">
-        <v>1</v>
-      </c>
-      <c r="F37" s="32">
+      <c r="C37" s="29"/>
+      <c r="E37" s="33">
+        <v>1</v>
+      </c>
+      <c r="F37" s="29">
         <v>0</v>
       </c>
-      <c r="G37" s="32"/>
+      <c r="G37" s="29"/>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="2" t="s">
@@ -7021,16 +7020,16 @@
       <c r="B38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="37">
-        <v>1</v>
-      </c>
-      <c r="F38" s="32">
+      <c r="E38" s="33">
+        <v>1</v>
+      </c>
+      <c r="F38" s="29">
         <v>0</v>
       </c>
-      <c r="G38" s="32"/>
+      <c r="G38" s="29"/>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="2" t="s">
@@ -7039,38 +7038,38 @@
       <c r="B39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="37">
-        <v>1</v>
-      </c>
-      <c r="F39" s="32">
+      <c r="E39" s="33">
+        <v>1</v>
+      </c>
+      <c r="F39" s="29">
         <v>0</v>
       </c>
-      <c r="G39" s="32"/>
+      <c r="G39" s="29"/>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="32"/>
-      <c r="E40" s="32"/>
+      <c r="C40" s="29"/>
+      <c r="E40" s="29"/>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
-      <c r="E41" s="32"/>
+      <c r="E41" s="29"/>
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
-      <c r="E42" s="32"/>
+      <c r="E42" s="29"/>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="32"/>
-      <c r="E43" s="32"/>
+      <c r="C43" s="29"/>
+      <c r="E43" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7082,4 +7081,39 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="16.78125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>